<commit_message>
OMG Phase 1.5 complete system
</commit_message>
<xml_diff>
--- a/debug/ARB_debug.xlsx
+++ b/debug/ARB_debug.xlsx
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE1037"/>
+  <dimension ref="A1:AE1044"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -105335,13 +105335,13 @@
         <v>0.3093</v>
       </c>
       <c r="C1037" t="n">
-        <v>0.3189</v>
+        <v>0.3225</v>
       </c>
       <c r="D1037" t="n">
         <v>0.3043</v>
       </c>
       <c r="E1037" t="n">
-        <v>0.3125</v>
+        <v>0.3172</v>
       </c>
       <c r="F1037" t="inlineStr">
         <is>
@@ -105379,7 +105379,7 @@
         <v>0.2878</v>
       </c>
       <c r="Q1037" t="n">
-        <v>10.806115</v>
+        <v>12.056984</v>
       </c>
       <c r="R1037" t="n">
         <v>17.3</v>
@@ -105424,6 +105424,713 @@
       </c>
       <c r="AE1037" t="n">
         <v>0.3043</v>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>2025-10-19</t>
+        </is>
+      </c>
+      <c r="B1038" t="n">
+        <v>0.3172</v>
+      </c>
+      <c r="C1038" t="n">
+        <v>0.3288</v>
+      </c>
+      <c r="D1038" t="n">
+        <v>0.3103</v>
+      </c>
+      <c r="E1038" t="n">
+        <v>0.3221</v>
+      </c>
+      <c r="F1038" t="inlineStr">
+        <is>
+          <t>wait</t>
+        </is>
+      </c>
+      <c r="G1038" t="b">
+        <v>1</v>
+      </c>
+      <c r="H1038" t="n">
+        <v>2</v>
+      </c>
+      <c r="I1038" t="n">
+        <v/>
+      </c>
+      <c r="J1038" t="n">
+        <v/>
+      </c>
+      <c r="K1038" t="n">
+        <v/>
+      </c>
+      <c r="L1038" t="n">
+        <v/>
+      </c>
+      <c r="M1038" t="n">
+        <v/>
+      </c>
+      <c r="N1038" t="n">
+        <v/>
+      </c>
+      <c r="O1038" t="n">
+        <v>0.6246</v>
+      </c>
+      <c r="P1038" t="n">
+        <v>0.2878</v>
+      </c>
+      <c r="Q1038" t="n">
+        <v>14.246004</v>
+      </c>
+      <c r="R1038" t="n">
+        <v>17.3</v>
+      </c>
+      <c r="S1038" t="n">
+        <v>6</v>
+      </c>
+      <c r="T1038" t="n">
+        <v>0.349776</v>
+      </c>
+      <c r="U1038" t="n">
+        <v>0.324792</v>
+      </c>
+      <c r="V1038" t="n">
+        <v>0.287316</v>
+      </c>
+      <c r="W1038" t="n">
+        <v>0.256086</v>
+      </c>
+      <c r="X1038" t="n">
+        <v>0.21861</v>
+      </c>
+      <c r="Y1038" t="n">
+        <v>0.174888</v>
+      </c>
+      <c r="Z1038" t="n">
+        <v>0.131166</v>
+      </c>
+      <c r="AA1038" t="n">
+        <v>0.118674</v>
+      </c>
+      <c r="AB1038" t="n">
+        <v>0.3391143</v>
+      </c>
+      <c r="AC1038" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="AD1038" t="n">
+        <v>0.324792</v>
+      </c>
+      <c r="AE1038" t="n">
+        <v>0.3103</v>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>2025-10-20</t>
+        </is>
+      </c>
+      <c r="B1039" t="n">
+        <v>0.3221</v>
+      </c>
+      <c r="C1039" t="n">
+        <v>0.3353</v>
+      </c>
+      <c r="D1039" t="n">
+        <v>0.3087</v>
+      </c>
+      <c r="E1039" t="n">
+        <v>0.311</v>
+      </c>
+      <c r="F1039" t="inlineStr">
+        <is>
+          <t>wait</t>
+        </is>
+      </c>
+      <c r="G1039" t="b">
+        <v>1</v>
+      </c>
+      <c r="H1039" t="n">
+        <v>2</v>
+      </c>
+      <c r="I1039" t="n">
+        <v/>
+      </c>
+      <c r="J1039" t="n">
+        <v/>
+      </c>
+      <c r="K1039" t="n">
+        <v/>
+      </c>
+      <c r="L1039" t="n">
+        <v/>
+      </c>
+      <c r="M1039" t="n">
+        <v/>
+      </c>
+      <c r="N1039" t="n">
+        <v/>
+      </c>
+      <c r="O1039" t="n">
+        <v>0.6246</v>
+      </c>
+      <c r="P1039" t="n">
+        <v>0.2878</v>
+      </c>
+      <c r="Q1039" t="n">
+        <v>16.504517</v>
+      </c>
+      <c r="R1039" t="n">
+        <v>17.3</v>
+      </c>
+      <c r="S1039" t="n">
+        <v>6</v>
+      </c>
+      <c r="T1039" t="n">
+        <v>0.349776</v>
+      </c>
+      <c r="U1039" t="n">
+        <v>0.324792</v>
+      </c>
+      <c r="V1039" t="n">
+        <v>0.287316</v>
+      </c>
+      <c r="W1039" t="n">
+        <v>0.256086</v>
+      </c>
+      <c r="X1039" t="n">
+        <v>0.21861</v>
+      </c>
+      <c r="Y1039" t="n">
+        <v>0.174888</v>
+      </c>
+      <c r="Z1039" t="n">
+        <v>0.131166</v>
+      </c>
+      <c r="AA1039" t="n">
+        <v>0.118674</v>
+      </c>
+      <c r="AB1039" t="n">
+        <v>0.3391143</v>
+      </c>
+      <c r="AC1039" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="AD1039" t="n">
+        <v>0.324792</v>
+      </c>
+      <c r="AE1039" t="n">
+        <v>0.3087</v>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>2025-10-21</t>
+        </is>
+      </c>
+      <c r="B1040" t="n">
+        <v>0.3109</v>
+      </c>
+      <c r="C1040" t="n">
+        <v>0.3129</v>
+      </c>
+      <c r="D1040" t="n">
+        <v>0.2917</v>
+      </c>
+      <c r="E1040" t="n">
+        <v>0.3012</v>
+      </c>
+      <c r="F1040" t="inlineStr">
+        <is>
+          <t>wait</t>
+        </is>
+      </c>
+      <c r="G1040" t="b">
+        <v>1</v>
+      </c>
+      <c r="H1040" t="n">
+        <v>2</v>
+      </c>
+      <c r="I1040" t="n">
+        <v/>
+      </c>
+      <c r="J1040" t="n">
+        <v/>
+      </c>
+      <c r="K1040" t="n">
+        <v/>
+      </c>
+      <c r="L1040" t="n">
+        <v/>
+      </c>
+      <c r="M1040" t="n">
+        <v/>
+      </c>
+      <c r="N1040" t="n">
+        <v/>
+      </c>
+      <c r="O1040" t="n">
+        <v>0.6246</v>
+      </c>
+      <c r="P1040" t="n">
+        <v>0.2878</v>
+      </c>
+      <c r="Q1040" t="n">
+        <v>8.721334000000001</v>
+      </c>
+      <c r="R1040" t="n">
+        <v>17.3</v>
+      </c>
+      <c r="S1040" t="n">
+        <v>6</v>
+      </c>
+      <c r="T1040" t="n">
+        <v>0.349776</v>
+      </c>
+      <c r="U1040" t="n">
+        <v>0.324792</v>
+      </c>
+      <c r="V1040" t="n">
+        <v>0.287316</v>
+      </c>
+      <c r="W1040" t="n">
+        <v>0.256086</v>
+      </c>
+      <c r="X1040" t="n">
+        <v>0.21861</v>
+      </c>
+      <c r="Y1040" t="n">
+        <v>0.174888</v>
+      </c>
+      <c r="Z1040" t="n">
+        <v>0.131166</v>
+      </c>
+      <c r="AA1040" t="n">
+        <v>0.118674</v>
+      </c>
+      <c r="AB1040" t="n">
+        <v>0.3391143</v>
+      </c>
+      <c r="AC1040" t="inlineStr">
+        <is>
+          <t>B7</t>
+        </is>
+      </c>
+      <c r="AD1040" t="n">
+        <v>0.131166</v>
+      </c>
+      <c r="AE1040" t="n">
+        <v>0.2917</v>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>2025-10-22</t>
+        </is>
+      </c>
+      <c r="B1041" t="n">
+        <v>0.3012</v>
+      </c>
+      <c r="C1041" t="n">
+        <v>0.3196</v>
+      </c>
+      <c r="D1041" t="n">
+        <v>0.2999</v>
+      </c>
+      <c r="E1041" t="n">
+        <v>0.3141</v>
+      </c>
+      <c r="F1041" t="inlineStr">
+        <is>
+          <t>wait</t>
+        </is>
+      </c>
+      <c r="G1041" t="b">
+        <v>1</v>
+      </c>
+      <c r="H1041" t="n">
+        <v>2</v>
+      </c>
+      <c r="I1041" t="n">
+        <v/>
+      </c>
+      <c r="J1041" t="n">
+        <v/>
+      </c>
+      <c r="K1041" t="n">
+        <v/>
+      </c>
+      <c r="L1041" t="n">
+        <v/>
+      </c>
+      <c r="M1041" t="n">
+        <v/>
+      </c>
+      <c r="N1041" t="n">
+        <v/>
+      </c>
+      <c r="O1041" t="n">
+        <v>0.6246</v>
+      </c>
+      <c r="P1041" t="n">
+        <v>0.2878</v>
+      </c>
+      <c r="Q1041" t="n">
+        <v>11.04934</v>
+      </c>
+      <c r="R1041" t="n">
+        <v>17.3</v>
+      </c>
+      <c r="S1041" t="n">
+        <v>6</v>
+      </c>
+      <c r="T1041" t="n">
+        <v>0.349776</v>
+      </c>
+      <c r="U1041" t="n">
+        <v>0.324792</v>
+      </c>
+      <c r="V1041" t="n">
+        <v>0.287316</v>
+      </c>
+      <c r="W1041" t="n">
+        <v>0.256086</v>
+      </c>
+      <c r="X1041" t="n">
+        <v>0.21861</v>
+      </c>
+      <c r="Y1041" t="n">
+        <v>0.174888</v>
+      </c>
+      <c r="Z1041" t="n">
+        <v>0.131166</v>
+      </c>
+      <c r="AA1041" t="n">
+        <v>0.118674</v>
+      </c>
+      <c r="AB1041" t="n">
+        <v>0.3391143</v>
+      </c>
+      <c r="AC1041" t="inlineStr">
+        <is>
+          <t>B7</t>
+        </is>
+      </c>
+      <c r="AD1041" t="n">
+        <v>0.131166</v>
+      </c>
+      <c r="AE1041" t="n">
+        <v>0.2999</v>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>2025-10-23</t>
+        </is>
+      </c>
+      <c r="B1042" t="n">
+        <v>0.3141</v>
+      </c>
+      <c r="C1042" t="n">
+        <v>0.3246</v>
+      </c>
+      <c r="D1042" t="n">
+        <v>0.3116</v>
+      </c>
+      <c r="E1042" t="n">
+        <v>0.3202</v>
+      </c>
+      <c r="F1042" t="inlineStr">
+        <is>
+          <t>wait</t>
+        </is>
+      </c>
+      <c r="G1042" t="b">
+        <v>1</v>
+      </c>
+      <c r="H1042" t="n">
+        <v>2</v>
+      </c>
+      <c r="I1042" t="n">
+        <v/>
+      </c>
+      <c r="J1042" t="n">
+        <v/>
+      </c>
+      <c r="K1042" t="n">
+        <v/>
+      </c>
+      <c r="L1042" t="n">
+        <v/>
+      </c>
+      <c r="M1042" t="n">
+        <v/>
+      </c>
+      <c r="N1042" t="n">
+        <v/>
+      </c>
+      <c r="O1042" t="n">
+        <v>0.6246</v>
+      </c>
+      <c r="P1042" t="n">
+        <v>0.2878</v>
+      </c>
+      <c r="Q1042" t="n">
+        <v>12.786657</v>
+      </c>
+      <c r="R1042" t="n">
+        <v>17.3</v>
+      </c>
+      <c r="S1042" t="n">
+        <v>6</v>
+      </c>
+      <c r="T1042" t="n">
+        <v>0.349776</v>
+      </c>
+      <c r="U1042" t="n">
+        <v>0.324792</v>
+      </c>
+      <c r="V1042" t="n">
+        <v>0.287316</v>
+      </c>
+      <c r="W1042" t="n">
+        <v>0.256086</v>
+      </c>
+      <c r="X1042" t="n">
+        <v>0.21861</v>
+      </c>
+      <c r="Y1042" t="n">
+        <v>0.174888</v>
+      </c>
+      <c r="Z1042" t="n">
+        <v>0.131166</v>
+      </c>
+      <c r="AA1042" t="n">
+        <v>0.118674</v>
+      </c>
+      <c r="AB1042" t="n">
+        <v>0.3391143</v>
+      </c>
+      <c r="AC1042" t="inlineStr">
+        <is>
+          <t>B7</t>
+        </is>
+      </c>
+      <c r="AD1042" t="n">
+        <v>0.131166</v>
+      </c>
+      <c r="AE1042" t="n">
+        <v>0.3116</v>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>2025-10-24</t>
+        </is>
+      </c>
+      <c r="B1043" t="n">
+        <v>0.3201</v>
+      </c>
+      <c r="C1043" t="n">
+        <v>0.3226</v>
+      </c>
+      <c r="D1043" t="n">
+        <v>0.3167</v>
+      </c>
+      <c r="E1043" t="n">
+        <v>0.3203</v>
+      </c>
+      <c r="F1043" t="inlineStr">
+        <is>
+          <t>wait</t>
+        </is>
+      </c>
+      <c r="G1043" t="b">
+        <v>1</v>
+      </c>
+      <c r="H1043" t="n">
+        <v>2</v>
+      </c>
+      <c r="I1043" t="n">
+        <v/>
+      </c>
+      <c r="J1043" t="n">
+        <v/>
+      </c>
+      <c r="K1043" t="n">
+        <v/>
+      </c>
+      <c r="L1043" t="n">
+        <v/>
+      </c>
+      <c r="M1043" t="n">
+        <v/>
+      </c>
+      <c r="N1043" t="n">
+        <v/>
+      </c>
+      <c r="O1043" t="n">
+        <v>0.6246</v>
+      </c>
+      <c r="P1043" t="n">
+        <v>0.2878</v>
+      </c>
+      <c r="Q1043" t="n">
+        <v>12.09173</v>
+      </c>
+      <c r="R1043" t="n">
+        <v>17.3</v>
+      </c>
+      <c r="S1043" t="n">
+        <v>6</v>
+      </c>
+      <c r="T1043" t="n">
+        <v>0.349776</v>
+      </c>
+      <c r="U1043" t="n">
+        <v>0.324792</v>
+      </c>
+      <c r="V1043" t="n">
+        <v>0.287316</v>
+      </c>
+      <c r="W1043" t="n">
+        <v>0.256086</v>
+      </c>
+      <c r="X1043" t="n">
+        <v>0.21861</v>
+      </c>
+      <c r="Y1043" t="n">
+        <v>0.174888</v>
+      </c>
+      <c r="Z1043" t="n">
+        <v>0.131166</v>
+      </c>
+      <c r="AA1043" t="n">
+        <v>0.118674</v>
+      </c>
+      <c r="AB1043" t="n">
+        <v>0.3391143</v>
+      </c>
+      <c r="AC1043" t="inlineStr">
+        <is>
+          <t>B7</t>
+        </is>
+      </c>
+      <c r="AD1043" t="n">
+        <v>0.131166</v>
+      </c>
+      <c r="AE1043" t="n">
+        <v>0.3167</v>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>2025-10-25</t>
+        </is>
+      </c>
+      <c r="B1044" t="n">
+        <v>0.3203</v>
+      </c>
+      <c r="C1044" t="n">
+        <v>0.3321</v>
+      </c>
+      <c r="D1044" t="n">
+        <v>0.3143</v>
+      </c>
+      <c r="E1044" t="n">
+        <v>0.3294</v>
+      </c>
+      <c r="F1044" t="inlineStr">
+        <is>
+          <t>wait</t>
+        </is>
+      </c>
+      <c r="G1044" t="b">
+        <v>1</v>
+      </c>
+      <c r="H1044" t="n">
+        <v>2</v>
+      </c>
+      <c r="I1044" t="n">
+        <v/>
+      </c>
+      <c r="J1044" t="n">
+        <v/>
+      </c>
+      <c r="K1044" t="n">
+        <v/>
+      </c>
+      <c r="L1044" t="n">
+        <v/>
+      </c>
+      <c r="M1044" t="n">
+        <v/>
+      </c>
+      <c r="N1044" t="n">
+        <v/>
+      </c>
+      <c r="O1044" t="n">
+        <v>0.6246</v>
+      </c>
+      <c r="P1044" t="n">
+        <v>0.2878</v>
+      </c>
+      <c r="Q1044" t="n">
+        <v>15.392634</v>
+      </c>
+      <c r="R1044" t="n">
+        <v>17.3</v>
+      </c>
+      <c r="S1044" t="n">
+        <v>6</v>
+      </c>
+      <c r="T1044" t="n">
+        <v>0.349776</v>
+      </c>
+      <c r="U1044" t="n">
+        <v>0.324792</v>
+      </c>
+      <c r="V1044" t="n">
+        <v>0.287316</v>
+      </c>
+      <c r="W1044" t="n">
+        <v>0.256086</v>
+      </c>
+      <c r="X1044" t="n">
+        <v>0.21861</v>
+      </c>
+      <c r="Y1044" t="n">
+        <v>0.174888</v>
+      </c>
+      <c r="Z1044" t="n">
+        <v>0.131166</v>
+      </c>
+      <c r="AA1044" t="n">
+        <v>0.118674</v>
+      </c>
+      <c r="AB1044" t="n">
+        <v>0.3391143</v>
+      </c>
+      <c r="AC1044" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="AD1044" t="n">
+        <v>0.324792</v>
+      </c>
+      <c r="AE1044" t="n">
+        <v>0.3143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>